<commit_message>
📄 Normal update: 90 articles from 9 tags
</commit_message>
<xml_diff>
--- a/data/news_2026-02-03.xlsx
+++ b/data/news_2026-02-03.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G21"/>
+  <dimension ref="A1:G111"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -885,9 +885,2079 @@
         <v>2026-02-03T08:46:10.670Z</v>
       </c>
     </row>
+    <row r="22">
+      <c r="A22" t="str">
+        <v>金银矿产业链</v>
+      </c>
+      <c r="B22" t="str">
+        <v>https://www.zerohedge.com/markets/stocks-slide-gold-and-bitcoin-tumble-after-trump-taps-warsh-next-fed-chair</v>
+      </c>
+      <c r="C22" t="str">
+        <v>Stocks Slide, Gold And Bitcoin Tumble After Trump Taps Warsh As Next Fed Chair</v>
+      </c>
+      <c r="D22" t="str">
+        <v>特朗普提名沃什为下任美联储主席后，股市下跌，黄金和比特币暴跌，反映市场对货币政策走向的担忧。</v>
+      </c>
+      <c r="E22">
+        <v>4</v>
+      </c>
+      <c r="F22" t="str">
+        <v>normal</v>
+      </c>
+      <c r="G22" t="str">
+        <v>2026-02-03T10:56:10.149Z</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="str">
+        <v>金银矿产业链</v>
+      </c>
+      <c r="B23" t="str">
+        <v>https://www.zerohedge.com/markets/stocks-slide-gold-and-bitcoin-tumble-after-trump-taps-warsh-next-fed-chair</v>
+      </c>
+      <c r="C23" t="str">
+        <v>Stocks Slide, Gold And Bitcoin Tumble After Trump Taps Warsh As Next Fed Chair</v>
+      </c>
+      <c r="D23" t="str">
+        <v>特朗普可能任命Warsh为下一任美联储主席引发市场动荡，股市下跌，黄金和比特币暴跌。</v>
+      </c>
+      <c r="E23">
+        <v>4</v>
+      </c>
+      <c r="F23" t="str">
+        <v>normal</v>
+      </c>
+      <c r="G23" t="str">
+        <v>2026-02-03T10:56:10.149Z</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="str">
+        <v>金银矿产业链</v>
+      </c>
+      <c r="B24" t="str">
+        <v>https://www.zerohedge.com/precious-metals/expect-precious-metals-rally-continue-2026</v>
+      </c>
+      <c r="C24" t="str">
+        <v>Expect The Precious Metals Rally To Continue In 2026</v>
+      </c>
+      <c r="D24" t="str">
+        <v>预计贵金属涨势将持续到2026年，具体原因和来源未知，需谨慎参考。</v>
+      </c>
+      <c r="E24">
+        <v>2</v>
+      </c>
+      <c r="F24" t="str">
+        <v>normal</v>
+      </c>
+      <c r="G24" t="str">
+        <v>2026-02-03T10:56:10.149Z</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="str">
+        <v>金银矿产业链</v>
+      </c>
+      <c r="B25" t="str">
+        <v>https://www.zerohedge.com/markets/stocks-head-first-drop-2026-focus-turns-geopolitics-macro</v>
+      </c>
+      <c r="C25" t="str">
+        <v>Stocks Head For First Drop Of 2026 As Focus Turns To Geopolitics, Macro</v>
+      </c>
+      <c r="D25" t="str">
+        <v>地缘政治和宏观经济担忧导致股市下跌，或为2026年首次下跌。</v>
+      </c>
+      <c r="E25">
+        <v>4</v>
+      </c>
+      <c r="F25" t="str">
+        <v>normal</v>
+      </c>
+      <c r="G25" t="str">
+        <v>2026-02-03T10:56:10.149Z</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="str">
+        <v>金银矿产业链</v>
+      </c>
+      <c r="B26" t="str">
+        <v>https://www.zerohedge.com/markets/stocks-head-first-drop-2026-focus-turns-geopolitics-macro</v>
+      </c>
+      <c r="C26" t="str">
+        <v>Stocks Head For First Drop Of 2026 As Focus Turns To Geopolitics, Macro</v>
+      </c>
+      <c r="D26" t="str">
+        <v>地缘政治和宏观经济因素导致股市可能在2026年首次下跌。</v>
+      </c>
+      <c r="E26">
+        <v>4</v>
+      </c>
+      <c r="F26" t="str">
+        <v>normal</v>
+      </c>
+      <c r="G26" t="str">
+        <v>2026-02-03T10:56:10.149Z</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="str">
+        <v>金银矿产业链</v>
+      </c>
+      <c r="B27" t="str">
+        <v>https://www.zerohedge.com/markets/us-equity-futures-jump-record-high-after-core-cpi-comes-cool</v>
+      </c>
+      <c r="C27" t="str">
+        <v>US Equity Futures Jump To Record High After Core CPI Comes In Cool</v>
+      </c>
+      <c r="D27" t="str">
+        <v>美国核心CPI数据低于预期，美股期货飙升至历史新高，市场乐观情绪高涨。</v>
+      </c>
+      <c r="E27">
+        <v>4</v>
+      </c>
+      <c r="F27" t="str">
+        <v>normal</v>
+      </c>
+      <c r="G27" t="str">
+        <v>2026-02-03T10:56:10.149Z</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="str">
+        <v>金银矿产业链</v>
+      </c>
+      <c r="B28" t="str">
+        <v>https://www.zerohedge.com/geopolitical/trump-kicking-brics-out-americas</v>
+      </c>
+      <c r="C28" t="str">
+        <v>Trump Kicking BRICS Out Of The Americas</v>
+      </c>
+      <c r="D28" t="str">
+        <v>据称特朗普计划将金砖国家从美洲地区驱逐，可能引发地缘政治和贸易紧张。（如果消息属实）</v>
+      </c>
+      <c r="E28">
+        <v>4</v>
+      </c>
+      <c r="F28" t="str">
+        <v>normal</v>
+      </c>
+      <c r="G28" t="str">
+        <v>2026-02-03T10:56:10.149Z</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="str">
+        <v>金银矿产业链</v>
+      </c>
+      <c r="B29" t="str">
+        <v>https://www.zerohedge.com/geopolitical/30-ways-trump-impacted-world-his-first-year</v>
+      </c>
+      <c r="C29" t="str">
+        <v>30 Ways Trump Impacted The World In His First Year</v>
+      </c>
+      <c r="D29" t="str">
+        <v>该文章列举了特朗普执政第一年对世界产生的30个方面的影响，涵盖政策、国际关系等。</v>
+      </c>
+      <c r="E29">
+        <v>4</v>
+      </c>
+      <c r="F29" t="str">
+        <v>normal</v>
+      </c>
+      <c r="G29" t="str">
+        <v>2026-02-03T10:56:10.149Z</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="str">
+        <v>金银矿产业链</v>
+      </c>
+      <c r="B30" t="str">
+        <v>https://www.rt.com/business/631301-gold-reserves-cbr-gosfund/?utm_source=rss&amp;utm_medium=rss&amp;utm_campaign=RSS</v>
+      </c>
+      <c r="C30" t="str">
+        <v>Buckets and bullion: Behind the glitter of Russia’s gold reserves</v>
+      </c>
+      <c r="D30" t="str">
+        <v>文章揭示俄罗斯黄金储备的构成、管理和地缘政治意义，或涉及其在应对制裁中的作用。</v>
+      </c>
+      <c r="E30">
+        <v>4</v>
+      </c>
+      <c r="F30" t="str">
+        <v>normal</v>
+      </c>
+      <c r="G30" t="str">
+        <v>2026-02-03T10:56:10.149Z</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="str">
+        <v>金银矿产业链</v>
+      </c>
+      <c r="B31" t="str">
+        <v>https://www.rt.com/business/631301-gold-reserves-cbr-gosfund/?utm_source=rss&amp;utm_medium=rss&amp;utm_campaign=RSS</v>
+      </c>
+      <c r="C31" t="str">
+        <v>Buckets and bullion: Behind the glitter of Russia’s gold reserves</v>
+      </c>
+      <c r="D31" t="str">
+        <v>文章揭示俄罗斯黄金储备的构成、存储和作用，或分析其在地缘政治和经济中的战略意义。</v>
+      </c>
+      <c r="E31">
+        <v>4</v>
+      </c>
+      <c r="F31" t="str">
+        <v>normal</v>
+      </c>
+      <c r="G31" t="str">
+        <v>2026-02-03T10:56:10.149Z</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="str">
+        <v>黄金-美元-利率</v>
+      </c>
+      <c r="B32" t="str">
+        <v>https://in-cyprus.philenews.com/insider/european-shares-flat-as-defensives-limit-commodities-slump/</v>
+      </c>
+      <c r="C32" t="str">
+        <v>European shares flat as defensives limit commodities slump</v>
+      </c>
+      <c r="D32" t="str">
+        <v>欧洲股市持平，防御性股票限制了大宗商品下跌的影响，市场情绪谨慎。</v>
+      </c>
+      <c r="E32">
+        <v>3</v>
+      </c>
+      <c r="F32" t="str">
+        <v>normal</v>
+      </c>
+      <c r="G32" t="str">
+        <v>2026-02-03T10:56:10.149Z</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="str">
+        <v>黄金-美元-利率</v>
+      </c>
+      <c r="B33" t="str">
+        <v>https://www.theguardian.com/business/2026/feb/02/plunge-in-price-of-gold-and-silver-rattles-global-stock-markets</v>
+      </c>
+      <c r="C33" t="str">
+        <v>Plunge in price of gold and silver rattles global stock markets</v>
+      </c>
+      <c r="D33" t="str">
+        <v>金银价格暴跌引发全球股市动荡，投资者避险情绪或受影响。</v>
+      </c>
+      <c r="E33">
+        <v>4</v>
+      </c>
+      <c r="F33" t="str">
+        <v>normal</v>
+      </c>
+      <c r="G33" t="str">
+        <v>2026-02-03T10:56:10.149Z</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="str">
+        <v>黄金-美元-利率</v>
+      </c>
+      <c r="B34" t="str">
+        <v>https://www.zerohedge.com/markets/bitcoin-crashes-nov-2024-lows-amid-15-billion-levered-liquidations</v>
+      </c>
+      <c r="C34" t="str">
+        <v>Bitcoin Crashes To Nov 2024 Lows Amid $1.5 Billion In Levered Liquidations</v>
+      </c>
+      <c r="D34" t="str">
+        <v>比特币暴跌至2024年11月低点，引发15亿美元杠杆清算，市场剧烈波动。</v>
+      </c>
+      <c r="E34">
+        <v>4</v>
+      </c>
+      <c r="F34" t="str">
+        <v>normal</v>
+      </c>
+      <c r="G34" t="str">
+        <v>2026-02-03T10:56:10.149Z</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="str">
+        <v>黄金-美元-利率</v>
+      </c>
+      <c r="B35" t="str">
+        <v>https://finance.yahoo.com/news/fed-sends-surprising-message-gold-224700252.html</v>
+      </c>
+      <c r="C35" t="str">
+        <v>Fed sends surprising message on gold and silver price surge</v>
+      </c>
+      <c r="D35" t="str">
+        <v>分析失败</v>
+      </c>
+      <c r="E35" t="str">
+        <v/>
+      </c>
+      <c r="F35" t="str">
+        <v>normal</v>
+      </c>
+      <c r="G35" t="str">
+        <v>2026-02-03T10:56:10.149Z</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="str">
+        <v>黄金-美元-利率</v>
+      </c>
+      <c r="B36" t="str">
+        <v>https://www.bloomberg.com/news/videos/2026-01-30/bloomberg-businessweek-daily-1-30-2026-video</v>
+      </c>
+      <c r="C36" t="str">
+        <v>Trump Taps Warsh From 'Central Casting' For Fed | Bloomberg Businessweek Daily 1/30/2026</v>
+      </c>
+      <c r="D36" t="str">
+        <v>特朗普总统提名华尔街资深人士沃什担任美联储要职，引发市场对货币政策走向的关注。</v>
+      </c>
+      <c r="E36">
+        <v>4</v>
+      </c>
+      <c r="F36" t="str">
+        <v>normal</v>
+      </c>
+      <c r="G36" t="str">
+        <v>2026-02-03T10:56:10.149Z</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="str">
+        <v>黄金-美元-利率</v>
+      </c>
+      <c r="B37" t="str">
+        <v>https://finance.yahoo.com/news/gold-silver-surge-as-assault-on-fed-sparks-rush-to-precious-metals-151113516.html</v>
+      </c>
+      <c r="C37" t="str">
+        <v>Gold, silver surge as 'assault on Fed' sparks rush to precious metals</v>
+      </c>
+      <c r="D37" t="str">
+        <v>对美联储政策的质疑引发贵金属投资热潮，黄金和白银价格大幅上涨。</v>
+      </c>
+      <c r="E37">
+        <v>4</v>
+      </c>
+      <c r="F37" t="str">
+        <v>normal</v>
+      </c>
+      <c r="G37" t="str">
+        <v>2026-02-03T10:56:10.149Z</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="str">
+        <v>黄金-美元-利率</v>
+      </c>
+      <c r="B38" t="str">
+        <v>https://www.marketwatch.com/story/what-the-surge-in-gold-and-silver-to-fresh-records-says-about-the-mindset-of-investors-to-start-2026-f0b286b8?mod=mw_rss_topstories</v>
+      </c>
+      <c r="C38" t="str">
+        <v>What the surge in gold and silver to fresh records says about the mindset of investors to start 2026</v>
+      </c>
+      <c r="D38" t="str">
+        <v>金银价格创新高反映投资者对2026年初经济前景的担忧和避险情绪，或预示市场潜在风险。</v>
+      </c>
+      <c r="E38">
+        <v>4</v>
+      </c>
+      <c r="F38" t="str">
+        <v>normal</v>
+      </c>
+      <c r="G38" t="str">
+        <v>2026-02-03T10:56:10.149Z</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="str">
+        <v>黄金-美元-利率</v>
+      </c>
+      <c r="B39" t="str">
+        <v>https://www.marketwatch.com/story/these-6-reasons-for-golds-surge-are-keeping-investors-bullish-37cb3a45?mod=mw_rss_topstories</v>
+      </c>
+      <c r="C39" t="str">
+        <v>These 6 reasons for gold’s surge are keeping investors bullish</v>
+      </c>
+      <c r="D39" t="str">
+        <v>六大因素推动黄金价格上涨，投资者看涨情绪高涨，反映避险需求和通胀预期。</v>
+      </c>
+      <c r="E39">
+        <v>4</v>
+      </c>
+      <c r="F39" t="str">
+        <v>normal</v>
+      </c>
+      <c r="G39" t="str">
+        <v>2026-02-03T10:56:10.149Z</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="str">
+        <v>黄金-美元-利率</v>
+      </c>
+      <c r="B40" t="str">
+        <v>https://www.marketwatch.com/story/these-6-reasons-for-golds-surge-are-keeping-investors-bullish-37cb3a45?mod=mw_rss_topstories</v>
+      </c>
+      <c r="C40" t="str">
+        <v>Inflation fighter? Risk hedge? Why gold investors shouldn’t believe all they hear.</v>
+      </c>
+      <c r="D40" t="str">
+        <v>文章质疑了黄金作为对抗通胀和避险工具的传统观点，提醒投资者不要盲目听信宣传。</v>
+      </c>
+      <c r="E40">
+        <v>3</v>
+      </c>
+      <c r="F40" t="str">
+        <v>normal</v>
+      </c>
+      <c r="G40" t="str">
+        <v>2026-02-03T10:56:10.149Z</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="str">
+        <v>黄金-美元-利率</v>
+      </c>
+      <c r="B41" t="str">
+        <v>https://finance.yahoo.com/news/live/stock-market-today-dow-sp-500-eke-out-records-gold-soars-after-trump-amps-up-fight-with-fed-powell-210028506.html</v>
+      </c>
+      <c r="C41" t="str">
+        <v>Stock market today: Dow, S&amp;P 500 eke out records, gold soars after Trump amps up fight with Fed, Powell</v>
+      </c>
+      <c r="D41" t="str">
+        <v>特朗普加大与美联储的对抗，道琼斯和标普500指数创下纪录，黄金价格飙升。</v>
+      </c>
+      <c r="E41">
+        <v>4</v>
+      </c>
+      <c r="F41" t="str">
+        <v>normal</v>
+      </c>
+      <c r="G41" t="str">
+        <v>2026-02-03T10:56:10.149Z</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="str">
+        <v>macro-中国</v>
+      </c>
+      <c r="B42" t="str">
+        <v>https://www.zerohedge.com/markets/whats-warsh-could-happen</v>
+      </c>
+      <c r="C42" t="str">
+        <v>What's The Warsh That Could Happen?</v>
+      </c>
+      <c r="D42" t="str">
+        <v>文章标题暗示可能存在潜在冲突或危机，但具体内容未知，难以评估其影响。</v>
+      </c>
+      <c r="E42">
+        <v>2</v>
+      </c>
+      <c r="F42" t="str">
+        <v>normal</v>
+      </c>
+      <c r="G42" t="str">
+        <v>2026-02-03T10:56:10.149Z</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="str">
+        <v>macro-中国</v>
+      </c>
+      <c r="B43" t="str">
+        <v>https://www.rt.com/india/631866-balance-of-power-shifting-musk/?utm_source=rss&amp;utm_medium=rss&amp;utm_campaign=RSS</v>
+      </c>
+      <c r="C43" t="str">
+        <v>‘Balance of power shifting’ – Musk on India and China GDP growth</v>
+      </c>
+      <c r="D43" t="str">
+        <v>马斯克评论印度和中国GDP增长，暗示全球力量平衡正在转移。</v>
+      </c>
+      <c r="E43">
+        <v>4</v>
+      </c>
+      <c r="F43" t="str">
+        <v>normal</v>
+      </c>
+      <c r="G43" t="str">
+        <v>2026-02-03T10:56:10.149Z</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="str">
+        <v>macro-中国</v>
+      </c>
+      <c r="B44" t="str">
+        <v>https://www.rt.com/news/631769-dmitry-trenin-trumps-nds-2026/?utm_source=rss&amp;utm_medium=rss&amp;utm_campaign=RSS</v>
+      </c>
+      <c r="C44" t="str">
+        <v>Dmitry Trenin: America First goes global</v>
+      </c>
+      <c r="D44" t="str">
+        <v>德米特里·特列宁认为“美国优先”政策正在全球范围内蔓延，可能影响国际关系和地缘政治格局。</v>
+      </c>
+      <c r="E44">
+        <v>4</v>
+      </c>
+      <c r="F44" t="str">
+        <v>normal</v>
+      </c>
+      <c r="G44" t="str">
+        <v>2026-02-03T10:56:10.149Z</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="str">
+        <v>macro-中国</v>
+      </c>
+      <c r="B45" t="str">
+        <v>https://www.zerohedge.com/markets/japanese-yields-soar-all-time-high-after-pm-takaichi-calls-snap-election-seeking-more</v>
+      </c>
+      <c r="C45" t="str">
+        <v>Japanese Yields Soar To All Time High After PM Takaichi Calls Snap Election Seeking More Spending, Less Taxes</v>
+      </c>
+      <c r="D45" t="str">
+        <v>日本首相高市暗示提前大选，主张增加支出和减少税收，导致日本国债收益率飙升至历史新高。</v>
+      </c>
+      <c r="E45">
+        <v>4</v>
+      </c>
+      <c r="F45" t="str">
+        <v>normal</v>
+      </c>
+      <c r="G45" t="str">
+        <v>2026-02-03T10:56:10.149Z</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="str">
+        <v>macro-中国</v>
+      </c>
+      <c r="B46" t="str">
+        <v>https://www.zerohedge.com/markets/japanese-yields-soar-all-time-high-after-pm-takaichi-calls-snap-election-seeking-more</v>
+      </c>
+      <c r="C46" t="str">
+        <v>Japanese Yields Soar To All Time High After PM Takaichi Calls Snap Election Seeking More Spending, Less Taxes</v>
+      </c>
+      <c r="D46" t="str">
+        <v>日本首相高市呼吁提前大选，主张增加支出、减少税收，导致日本国债收益率飙升至历史新高。</v>
+      </c>
+      <c r="E46">
+        <v>4</v>
+      </c>
+      <c r="F46" t="str">
+        <v>normal</v>
+      </c>
+      <c r="G46" t="str">
+        <v>2026-02-03T10:56:10.149Z</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="str">
+        <v>macro-中国</v>
+      </c>
+      <c r="B47" t="str">
+        <v>https://www.zerohedge.com/political/much-defiance-no-strategy-germanys-outrage-trumps-greenland-policy</v>
+      </c>
+      <c r="C47" t="str">
+        <v>Much Defiance, No Strategy: Germany's Outrage At Trump's Greenland Policy</v>
+      </c>
+      <c r="D47" t="str">
+        <v>德国强烈谴责特朗普的格陵兰政策，但缺乏应对策略，显示出德国的被动反应。</v>
+      </c>
+      <c r="E47">
+        <v>3</v>
+      </c>
+      <c r="F47" t="str">
+        <v>normal</v>
+      </c>
+      <c r="G47" t="str">
+        <v>2026-02-03T10:56:10.149Z</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="str">
+        <v>macro-中国</v>
+      </c>
+      <c r="B48" t="str">
+        <v>https://www.zerohedge.com/political/much-defiance-no-strategy-germanys-outrage-trumps-greenland-policy</v>
+      </c>
+      <c r="C48" t="str">
+        <v>Much Defiance, No Strategy: Germany's Outrage At Trump's Greenland Policy</v>
+      </c>
+      <c r="D48" t="str">
+        <v>德国强烈谴责特朗普的格陵兰政策，但缺乏明确的应对策略，显示欧美关系紧张。</v>
+      </c>
+      <c r="E48">
+        <v>4</v>
+      </c>
+      <c r="F48" t="str">
+        <v>normal</v>
+      </c>
+      <c r="G48" t="str">
+        <v>2026-02-03T10:56:10.149Z</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="str">
+        <v>macro-中国</v>
+      </c>
+      <c r="B49" t="str">
+        <v>https://www.zerohedge.com/geopolitical/escobar-real-rupture-davos</v>
+      </c>
+      <c r="C49" t="str">
+        <v>Escobar: The Real "Rupture" In Davos</v>
+      </c>
+      <c r="D49" t="str">
+        <v>文章可能讨论了埃斯科巴尔事件对达沃斯论坛造成的实际影响或象征性冲击，暗示论坛的既定秩序或议题受到了挑战。</v>
+      </c>
+      <c r="E49">
+        <v>3</v>
+      </c>
+      <c r="F49" t="str">
+        <v>normal</v>
+      </c>
+      <c r="G49" t="str">
+        <v>2026-02-03T10:56:10.149Z</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="str">
+        <v>macro-中国</v>
+      </c>
+      <c r="B50" t="str">
+        <v>https://www.zerohedge.com/geopolitical/escobar-real-rupture-davos</v>
+      </c>
+      <c r="C50" t="str">
+        <v>Escobar: The Real "Rupture" In Davos</v>
+      </c>
+      <c r="D50" t="str">
+        <v>该文章可能探讨了埃斯科巴尔事件对达沃斯论坛造成的实际影响或象征性冲击，具体内容未知。</v>
+      </c>
+      <c r="E50">
+        <v>3</v>
+      </c>
+      <c r="F50" t="str">
+        <v>normal</v>
+      </c>
+      <c r="G50" t="str">
+        <v>2026-02-03T10:56:10.149Z</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="str">
+        <v>macro-中国</v>
+      </c>
+      <c r="B51" t="str">
+        <v>https://www.zerohedge.com/crypto/repricing-sovereignty</v>
+      </c>
+      <c r="C51" t="str">
+        <v>Repricing Sovereignty</v>
+      </c>
+      <c r="D51" t="str">
+        <v>主权重新定价可能涉及国家风险评估变化，影响国际投资和地缘政治格局，具体内容未知。</v>
+      </c>
+      <c r="E51">
+        <v>3</v>
+      </c>
+      <c r="F51" t="str">
+        <v>normal</v>
+      </c>
+      <c r="G51" t="str">
+        <v>2026-02-03T10:56:10.149Z</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="str">
+        <v>macro-美国</v>
+      </c>
+      <c r="B52" t="str">
+        <v>https://www.defensenews.com/global/europe/2026/02/02/russia-claims-15-billion-in-2025-arms-exports-with-focus-on-africa/</v>
+      </c>
+      <c r="C52" t="str">
+        <v>Russia claims $15 billion in 2025 arms exports, with focus on Africa</v>
+      </c>
+      <c r="D52" t="str">
+        <v>俄罗斯声称2025年武器出口额将达150亿美元，重点是非洲市场，表明其持续的军火贸易和地缘政治影响力。</v>
+      </c>
+      <c r="E52">
+        <v>4</v>
+      </c>
+      <c r="F52" t="str">
+        <v>normal</v>
+      </c>
+      <c r="G52" t="str">
+        <v>2026-02-03T10:56:10.149Z</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="str">
+        <v>macro-美国</v>
+      </c>
+      <c r="B53" t="str">
+        <v>https://www.rt.com/news/631769-dmitry-trenin-trumps-nds-2026/?utm_source=rss&amp;utm_medium=rss&amp;utm_campaign=RSS</v>
+      </c>
+      <c r="C53" t="str">
+        <v>Dmitry Trenin: America First goes global</v>
+      </c>
+      <c r="D53" t="str">
+        <v>德米特里·特列宁认为“美国优先”策略正在全球范围内被其他国家效仿，可能导致地缘政治格局变化。</v>
+      </c>
+      <c r="E53">
+        <v>4</v>
+      </c>
+      <c r="F53" t="str">
+        <v>normal</v>
+      </c>
+      <c r="G53" t="str">
+        <v>2026-02-03T10:56:10.149Z</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="str">
+        <v>macro-美国</v>
+      </c>
+      <c r="B54" t="str">
+        <v>https://www.rt.com/news/631772-nato-bank-prepare-russia-war/?utm_source=rss&amp;utm_medium=rss&amp;utm_campaign=RSS</v>
+      </c>
+      <c r="C54" t="str">
+        <v>NATO creating bank to prepare for war with Russia – media</v>
+      </c>
+      <c r="D54" t="str">
+        <v>据报道，北约正设立银行以应对与俄罗斯的潜在战争，此举或为加强防御和经济准备。</v>
+      </c>
+      <c r="E54">
+        <v>4</v>
+      </c>
+      <c r="F54" t="str">
+        <v>normal</v>
+      </c>
+      <c r="G54" t="str">
+        <v>2026-02-03T10:56:10.149Z</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="str">
+        <v>macro-美国</v>
+      </c>
+      <c r="B55" t="str">
+        <v>https://www.rt.com/news/631772-nato-bank-prepare-russia-war/?utm_source=rss&amp;utm_medium=rss&amp;utm_campaign=RSS</v>
+      </c>
+      <c r="C55" t="str">
+        <v>NATO creating bank to prepare for war with Russia – media</v>
+      </c>
+      <c r="D55" t="str">
+        <v>据报道，北约正设立银行以应对与俄罗斯的潜在战争，此举或旨在加强军事准备和经济韧性。</v>
+      </c>
+      <c r="E55">
+        <v>4</v>
+      </c>
+      <c r="F55" t="str">
+        <v>normal</v>
+      </c>
+      <c r="G55" t="str">
+        <v>2026-02-03T10:56:10.149Z</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="str">
+        <v>macro-美国</v>
+      </c>
+      <c r="B56" t="str">
+        <v>https://www.zerohedge.com/geopolitical/paleoconservative-rips-apart-trumps-venezuela-overthrow</v>
+      </c>
+      <c r="C56" t="str">
+        <v>A Paleoconservative Rips Apart Trump's Venezuela Overthrow</v>
+      </c>
+      <c r="D56" t="str">
+        <v>一位古保守派人士猛烈抨击了特朗普推翻委内瑞拉的企图，质疑其合法性和战略合理性。</v>
+      </c>
+      <c r="E56">
+        <v>3</v>
+      </c>
+      <c r="F56" t="str">
+        <v>normal</v>
+      </c>
+      <c r="G56" t="str">
+        <v>2026-02-03T10:56:10.149Z</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="str">
+        <v>macro-美国</v>
+      </c>
+      <c r="B57" t="str">
+        <v>https://www.zerohedge.com/political/bessent-reveals-10-us-budget-lost-fraud-signaling-musk-has-unfinished-doge-business</v>
+      </c>
+      <c r="C57" t="str">
+        <v>Bessent Reveals 10% Of US Budget Lost To Fraud, Signaling Musk Has Unfinished DOGE Business</v>
+      </c>
+      <c r="D57" t="str">
+        <v>Bessent声称美国预算10%因欺诈损失，暗示马斯克或将继续推动狗狗币发展，但信息来源不明，真实性待考。</v>
+      </c>
+      <c r="E57">
+        <v>3</v>
+      </c>
+      <c r="F57" t="str">
+        <v>normal</v>
+      </c>
+      <c r="G57" t="str">
+        <v>2026-02-03T10:56:10.149Z</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="str">
+        <v>macro-美国</v>
+      </c>
+      <c r="B58" t="str">
+        <v>https://www.zerohedge.com/personal-finance/forgotten-man</v>
+      </c>
+      <c r="C58" t="str">
+        <v>The Forgotten Man</v>
+      </c>
+      <c r="D58" t="str">
+        <v>文章可能探讨了被忽视的群体或个体，呼吁关注社会边缘人群的困境与需求。</v>
+      </c>
+      <c r="E58">
+        <v>3</v>
+      </c>
+      <c r="F58" t="str">
+        <v>normal</v>
+      </c>
+      <c r="G58" t="str">
+        <v>2026-02-03T10:56:10.149Z</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="str">
+        <v>macro-美国</v>
+      </c>
+      <c r="B59" t="str">
+        <v>https://www.zerohedge.com/geopolitical/how-brics-may-deliver-structural-shock-us-dollar-system</v>
+      </c>
+      <c r="C59" t="str">
+        <v>How BRICS May Deliver Structural Shock To US Dollar System</v>
+      </c>
+      <c r="D59" t="str">
+        <v>金砖国家可能通过贸易和金融合作挑战美元在全球金融体系中的主导地位，重塑国际经济格局。</v>
+      </c>
+      <c r="E59">
+        <v>4</v>
+      </c>
+      <c r="F59" t="str">
+        <v>normal</v>
+      </c>
+      <c r="G59" t="str">
+        <v>2026-02-03T10:56:10.149Z</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="str">
+        <v>macro-美国</v>
+      </c>
+      <c r="B60" t="str">
+        <v>https://www.zerohedge.com/geopolitical/how-brics-may-deliver-structural-shock-us-dollar-system</v>
+      </c>
+      <c r="C60" t="str">
+        <v>How BRICS May Deliver Structural Shock To US Dollar System</v>
+      </c>
+      <c r="D60" t="str">
+        <v>金砖国家可能通过挑战美元在国际贸易和金融中的主导地位，对美元体系造成结构性冲击。</v>
+      </c>
+      <c r="E60">
+        <v>4</v>
+      </c>
+      <c r="F60" t="str">
+        <v>normal</v>
+      </c>
+      <c r="G60" t="str">
+        <v>2026-02-03T10:56:10.149Z</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="str">
+        <v>macro-美国</v>
+      </c>
+      <c r="B61" t="str">
+        <v>https://www.zerohedge.com/geopolitical/leaked-internal-emails-show-berlin-greens-urged-deflect-blame-far-left-attack-power</v>
+      </c>
+      <c r="C61" t="str">
+        <v>Leaked Internal Emails Show Berlin Greens Urged To Deflect Blame From Far-Left Attack On Power Grid</v>
+      </c>
+      <c r="D61" t="str">
+        <v>泄露邮件显示，柏林绿党被敦促转移对极左势力袭击电网的指责，引发政治争议。</v>
+      </c>
+      <c r="E61">
+        <v>4</v>
+      </c>
+      <c r="F61" t="str">
+        <v>normal</v>
+      </c>
+      <c r="G61" t="str">
+        <v>2026-02-03T10:56:10.149Z</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="str">
+        <v>macro-欧洲</v>
+      </c>
+      <c r="B62" t="str">
+        <v>https://in-cyprus.philenews.com/insider/dollar-holds-gains-on-economic-data-fed-bets-aussie-jumps-on-rba-hike/</v>
+      </c>
+      <c r="C62" t="str">
+        <v>Dollar holds gains on economic data, Fed bets; Aussie jumps on RBA hike</v>
+      </c>
+      <c r="D62" t="str">
+        <v>美国经济数据和美联储预期提振美元，澳洲央行加息推动澳元上涨。</v>
+      </c>
+      <c r="E62">
+        <v>4</v>
+      </c>
+      <c r="F62" t="str">
+        <v>normal</v>
+      </c>
+      <c r="G62" t="str">
+        <v>2026-02-03T10:56:10.149Z</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="str">
+        <v>macro-欧洲</v>
+      </c>
+      <c r="B63" t="str">
+        <v>https://cyprus-mail.com/2026/02/01/cyprus-leads-eu-in-non-performing-government-loans</v>
+      </c>
+      <c r="C63" t="str">
+        <v>Cyprus leads EU in non-performing government loans</v>
+      </c>
+      <c r="D63" t="str">
+        <v>塞浦路斯政府不良贷款比例在欧盟中最高，表明其公共财政可能面临风险，或影响经济稳定。</v>
+      </c>
+      <c r="E63">
+        <v>4</v>
+      </c>
+      <c r="F63" t="str">
+        <v>normal</v>
+      </c>
+      <c r="G63" t="str">
+        <v>2026-02-03T10:56:10.149Z</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="str">
+        <v>macro-欧洲</v>
+      </c>
+      <c r="B64" t="str">
+        <v>https://cyprus-mail.com/2026/01/31/cyprus-business-now-gdp-forecast-unemployment-minimum-wage-gulf-ties-citea</v>
+      </c>
+      <c r="C64" t="str">
+        <v>Cyprus Business Now: GDP forecast, unemployment, minimum wage, Gulf ties, CITEA</v>
+      </c>
+      <c r="D64" t="str">
+        <v>分析失败</v>
+      </c>
+      <c r="E64" t="str">
+        <v/>
+      </c>
+      <c r="F64" t="str">
+        <v>normal</v>
+      </c>
+      <c r="G64" t="str">
+        <v>2026-02-03T10:56:10.149Z</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="str">
+        <v>macro-欧洲</v>
+      </c>
+      <c r="B65" t="str">
+        <v>https://cyprus-mail.com/2026/01/30/domestic-demand-set-to-drive-robust-economic-momentum-in-cyprus</v>
+      </c>
+      <c r="C65" t="str">
+        <v>Domestic demand set to drive robust economic momentum in Cyprus</v>
+      </c>
+      <c r="D65" t="str">
+        <v>塞浦路斯预计国内需求将推动强劲的经济增长势头，预示着该国经济前景乐观。</v>
+      </c>
+      <c r="E65">
+        <v>3</v>
+      </c>
+      <c r="F65" t="str">
+        <v>normal</v>
+      </c>
+      <c r="G65" t="str">
+        <v>2026-02-03T10:56:10.149Z</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="str">
+        <v>macro-欧洲</v>
+      </c>
+      <c r="B66" t="str">
+        <v>https://cyprus-mail.com/2026/01/30/domestic-demand-set-to-drive-robust-economic-momentum-in-cyprus</v>
+      </c>
+      <c r="C66" t="str">
+        <v>Domestic demand set to drive robust economic momentum in Cyprus</v>
+      </c>
+      <c r="D66" t="str">
+        <v>塞浦路斯预计国内需求将推动经济强劲增长，预示着该国经济前景乐观。</v>
+      </c>
+      <c r="E66">
+        <v>3</v>
+      </c>
+      <c r="F66" t="str">
+        <v>normal</v>
+      </c>
+      <c r="G66" t="str">
+        <v>2026-02-03T10:56:10.149Z</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="str">
+        <v>macro-欧洲</v>
+      </c>
+      <c r="B67" t="str">
+        <v>https://cyprus-mail.com/2026/01/15/cyprus-maintains-services-strength-despite-broader-eu-surplus-dip</v>
+      </c>
+      <c r="C67" t="str">
+        <v>Cyprus maintains services strength despite broader EU surplus dip</v>
+      </c>
+      <c r="D67" t="str">
+        <v>塞浦路斯在欧盟盈余普遍下降的情况下保持了服务业的优势，显示出其经济的韧性。</v>
+      </c>
+      <c r="E67">
+        <v>3</v>
+      </c>
+      <c r="F67" t="str">
+        <v>normal</v>
+      </c>
+      <c r="G67" t="str">
+        <v>2026-02-03T10:56:10.149Z</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="str">
+        <v>macro-欧洲</v>
+      </c>
+      <c r="B68" t="str">
+        <v>https://cyprus-mail.com/2026/01/16/cyprus-business-now-port-workers-real-estate-foreign-direct-investment-rescued-sinking-ship</v>
+      </c>
+      <c r="C68" t="str">
+        <v>Cyprus Business Now: port workers, real estate, foreign direct investment, rescued sinking ship</v>
+      </c>
+      <c r="D68" t="str">
+        <v>塞浦路斯经济新闻涉及港口工人、房地产、外国直接投资以及一艘沉船救援，反映了该国多元化的经济活动。</v>
+      </c>
+      <c r="E68">
+        <v>3</v>
+      </c>
+      <c r="F68" t="str">
+        <v>normal</v>
+      </c>
+      <c r="G68" t="str">
+        <v>2026-02-03T10:56:10.149Z</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="str">
+        <v>macro-欧洲</v>
+      </c>
+      <c r="B69" t="str">
+        <v>https://cyprus-mail.com/2026/01/17/cyprus-business-now-tourism-overnight-stays-finance-minister-cbc-renewables</v>
+      </c>
+      <c r="C69" t="str">
+        <v>Cyprus Business Now: tourism, overnight stays, Finance Minister, CBC, renewables</v>
+      </c>
+      <c r="D69" t="str">
+        <v>塞浦路斯商业新闻涵盖旅游业、过夜住宿、财政部长讲话、中央银行动态和可再生能源发展。</v>
+      </c>
+      <c r="E69">
+        <v>3</v>
+      </c>
+      <c r="F69" t="str">
+        <v>normal</v>
+      </c>
+      <c r="G69" t="str">
+        <v>2026-02-03T10:56:10.149Z</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="str">
+        <v>macro-欧洲</v>
+      </c>
+      <c r="B70" t="str">
+        <v>https://cyprus-mail.com/2026/01/18/cyprus-business-now-weekly-wrap-up-144</v>
+      </c>
+      <c r="C70" t="str">
+        <v>Cyprus Business Now: weekly wrap-up</v>
+      </c>
+      <c r="D70" t="str">
+        <v>塞浦路斯商业新闻周报总结了该岛国本周的商业动态，但具体内容未知。</v>
+      </c>
+      <c r="E70">
+        <v>2</v>
+      </c>
+      <c r="F70" t="str">
+        <v>normal</v>
+      </c>
+      <c r="G70" t="str">
+        <v>2026-02-03T10:56:10.149Z</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="str">
+        <v>macro-欧洲</v>
+      </c>
+      <c r="B71" t="str">
+        <v>https://cyprus-mail.com/2026/01/19/ecb-sees-inflation-stabilising-as-euro-area-enters-transition-phase</v>
+      </c>
+      <c r="C71" t="str">
+        <v>ECB sees inflation stabilising as euro area enters transition phase</v>
+      </c>
+      <c r="D71" t="str">
+        <v>欧洲央行认为欧元区进入转型期，通胀趋于稳定，但具体稳定程度和转型影响尚待观察。</v>
+      </c>
+      <c r="E71">
+        <v>4</v>
+      </c>
+      <c r="F71" t="str">
+        <v>normal</v>
+      </c>
+      <c r="G71" t="str">
+        <v>2026-02-03T10:56:10.149Z</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="str">
+        <v>tech</v>
+      </c>
+      <c r="B72" t="str">
+        <v>https://www.zerohedge.com/political/5-things-know-about-trumps-education-policy-rollout</v>
+      </c>
+      <c r="C72" t="str">
+        <v>5 Things To Know About Trump's Education Policy Rollout</v>
+      </c>
+      <c r="D72" t="str">
+        <v>新闻概述了特朗普教育政策的五个关键方面，可能涉及改革方向、资金分配或争议议题。</v>
+      </c>
+      <c r="E72">
+        <v>3</v>
+      </c>
+      <c r="F72" t="str">
+        <v>normal</v>
+      </c>
+      <c r="G72" t="str">
+        <v>2026-02-03T10:56:10.149Z</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="str">
+        <v>tech</v>
+      </c>
+      <c r="B73" t="str">
+        <v>https://www.zerohedge.com/technology/europes-ai-ambitions-threatened-soaring-memory-chip-prices</v>
+      </c>
+      <c r="C73" t="str">
+        <v>Europe's AI Ambitions Threatened By Soaring Memory Chip Prices</v>
+      </c>
+      <c r="D73" t="str">
+        <v>内存芯片价格飙升或将阻碍欧洲发展人工智能的雄心，提高AI开发成本并限制创新。</v>
+      </c>
+      <c r="E73">
+        <v>4</v>
+      </c>
+      <c r="F73" t="str">
+        <v>normal</v>
+      </c>
+      <c r="G73" t="str">
+        <v>2026-02-03T10:56:10.149Z</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="str">
+        <v>tech</v>
+      </c>
+      <c r="B74" t="str">
+        <v>https://www.zerohedge.com/markets/futures-drop-after-latest-trump-headline-vortex-silver-slides-ahead-index-rebalance</v>
+      </c>
+      <c r="C74" t="str">
+        <v>Futures Drop After Latest Trump Headline Vortex, Silver Slides Ahead Of Index Rebalance</v>
+      </c>
+      <c r="D74" t="str">
+        <v>分析失败</v>
+      </c>
+      <c r="E74" t="str">
+        <v/>
+      </c>
+      <c r="F74" t="str">
+        <v>normal</v>
+      </c>
+      <c r="G74" t="str">
+        <v>2026-02-03T10:56:10.149Z</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="str">
+        <v>tech</v>
+      </c>
+      <c r="B75" t="str">
+        <v>https://www.zerohedge.com/markets/futures-drop-after-latest-trump-headline-vortex-silver-slides-ahead-index-rebalance</v>
+      </c>
+      <c r="C75" t="str">
+        <v>Futures Drop After Latest Trump Headline Vortex, Silver Slides Ahead Of Index Rebalance</v>
+      </c>
+      <c r="D75" t="str">
+        <v>特朗普相关消息引发期货下跌，白银在指数再平衡前下跌。</v>
+      </c>
+      <c r="E75">
+        <v>3</v>
+      </c>
+      <c r="F75" t="str">
+        <v>normal</v>
+      </c>
+      <c r="G75" t="str">
+        <v>2026-02-03T10:56:10.149Z</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="str">
+        <v>tech</v>
+      </c>
+      <c r="B76" t="str">
+        <v>https://www.zerohedge.com/markets/us-equity-futures-jump-record-high-after-core-cpi-comes-cool</v>
+      </c>
+      <c r="C76" t="str">
+        <v>US Equity Futures Jump To Record High After Core CPI Comes In Cool</v>
+      </c>
+      <c r="D76" t="str">
+        <v>分析失败</v>
+      </c>
+      <c r="E76" t="str">
+        <v/>
+      </c>
+      <c r="F76" t="str">
+        <v>normal</v>
+      </c>
+      <c r="G76" t="str">
+        <v>2026-02-03T10:56:10.149Z</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="str">
+        <v>tech</v>
+      </c>
+      <c r="B77" t="str">
+        <v>https://www.zerohedge.com/markets/us-equity-futures-jump-record-high-after-core-cpi-comes-cool</v>
+      </c>
+      <c r="C77" t="str">
+        <v>US Equity Futures Jump To Record High After Core CPI Comes In Cool</v>
+      </c>
+      <c r="D77" t="str">
+        <v>美国核心CPI数据低于预期，美股期货飙升至历史新高，预示市场对通胀放缓的乐观情绪。</v>
+      </c>
+      <c r="E77">
+        <v>4</v>
+      </c>
+      <c r="F77" t="str">
+        <v>normal</v>
+      </c>
+      <c r="G77" t="str">
+        <v>2026-02-03T10:56:10.149Z</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="str">
+        <v>tech</v>
+      </c>
+      <c r="B78" t="str">
+        <v>https://www.scmp.com/tech/tech-trends/article/3339953/chinas-spacemit-launch-server-class-risc-v-processor-after-raising-us86-million?utm_source=rss_feed</v>
+      </c>
+      <c r="C78" t="str">
+        <v>China’s SpacemiT to launch server-class RISC-V processor after raising US$86 million</v>
+      </c>
+      <c r="D78" t="str">
+        <v>分析失败</v>
+      </c>
+      <c r="E78" t="str">
+        <v/>
+      </c>
+      <c r="F78" t="str">
+        <v>normal</v>
+      </c>
+      <c r="G78" t="str">
+        <v>2026-02-03T10:56:10.149Z</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="str">
+        <v>tech</v>
+      </c>
+      <c r="B79" t="str">
+        <v>https://focustaiwan.tw/business/202601150025</v>
+      </c>
+      <c r="C79" t="str">
+        <v>TSMC's Fab 2 in Arizona to begin mass production in 2nd half of 2027</v>
+      </c>
+      <c r="D79" t="str">
+        <v>台积电亚利桑那州Fab 2工厂预计2027下半年开始量产，增强美国芯片制造能力。</v>
+      </c>
+      <c r="E79">
+        <v>4</v>
+      </c>
+      <c r="F79" t="str">
+        <v>normal</v>
+      </c>
+      <c r="G79" t="str">
+        <v>2026-02-03T10:56:10.149Z</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="str">
+        <v>tech</v>
+      </c>
+      <c r="B80" t="str">
+        <v>https://www.zerohedge.com/political/big-bet-apprenticeships-frozen-labor-market</v>
+      </c>
+      <c r="C80" t="str">
+        <v>A Big Bet On Apprenticeships In A Frozen Labor Market</v>
+      </c>
+      <c r="D80" t="str">
+        <v>在劳动力市场低迷时期，该新闻关注对学徒制的重大投资，可能旨在解决技能差距和促进就业。</v>
+      </c>
+      <c r="E80">
+        <v>3</v>
+      </c>
+      <c r="F80" t="str">
+        <v>normal</v>
+      </c>
+      <c r="G80" t="str">
+        <v>2026-02-03T10:56:10.149Z</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="str">
+        <v>tech</v>
+      </c>
+      <c r="B81" t="str">
+        <v>https://www.zerohedge.com/geopolitical/30-ways-trump-impacted-world-his-first-year</v>
+      </c>
+      <c r="C81" t="str">
+        <v>30 Ways Trump Impacted The World In His First Year</v>
+      </c>
+      <c r="D81" t="str">
+        <v>文章列举了特朗普执政第一年对世界产生的30个方面的影响，涵盖政治、经济、社会等领域。</v>
+      </c>
+      <c r="E81">
+        <v>4</v>
+      </c>
+      <c r="F81" t="str">
+        <v>normal</v>
+      </c>
+      <c r="G81" t="str">
+        <v>2026-02-03T10:56:10.149Z</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="str">
+        <v>国家紧急</v>
+      </c>
+      <c r="B82" t="str">
+        <v>https://www.rt.com/russia/631902-ukraine-strike-novaya-kakhovka/?utm_source=rss&amp;utm_medium=rss&amp;utm_campaign=RSS</v>
+      </c>
+      <c r="C82" t="str">
+        <v>Three killed by Ukrainian artillery strike on Russian city – governor (PHOTO)</v>
+      </c>
+      <c r="D82" t="str">
+        <v>乌克兰炮击俄罗斯城市，造成三人死亡，州长已证实。</v>
+      </c>
+      <c r="E82">
+        <v>4</v>
+      </c>
+      <c r="F82" t="str">
+        <v>normal</v>
+      </c>
+      <c r="G82" t="str">
+        <v>2026-02-03T10:56:10.149Z</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="str">
+        <v>国家紧急</v>
+      </c>
+      <c r="B83" t="str">
+        <v>https://www.rt.com/russia/631902-ukraine-strike-novaya-kakhovka/?utm_source=rss&amp;utm_medium=rss&amp;utm_campaign=RSS</v>
+      </c>
+      <c r="C83" t="str">
+        <v>Three killed by Ukrainian artillery strike on Russian city – governor (PHOTO)</v>
+      </c>
+      <c r="D83" t="str">
+        <v>乌克兰炮击俄罗斯城市，导致三人死亡，州长已证实。（具体来源未知）</v>
+      </c>
+      <c r="E83">
+        <v>4</v>
+      </c>
+      <c r="F83" t="str">
+        <v>normal</v>
+      </c>
+      <c r="G83" t="str">
+        <v>2026-02-03T10:56:10.149Z</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="str">
+        <v>国家紧急</v>
+      </c>
+      <c r="B84" t="str">
+        <v>https://www.rt.com/russia/631902-ukraine-strike-novaya-kakhovka/?utm_source=rss&amp;utm_medium=rss&amp;utm_campaign=RSS</v>
+      </c>
+      <c r="C84" t="str">
+        <v>Three killed by Ukrainian artillery strike on Russian city – governor (PHOTO)</v>
+      </c>
+      <c r="D84" t="str">
+        <v>乌克兰炮击俄罗斯城市，造成三人死亡，州长已证实。</v>
+      </c>
+      <c r="E84">
+        <v>4</v>
+      </c>
+      <c r="F84" t="str">
+        <v>normal</v>
+      </c>
+      <c r="G84" t="str">
+        <v>2026-02-03T10:56:10.149Z</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="str">
+        <v>国家紧急</v>
+      </c>
+      <c r="B85" t="str">
+        <v>https://www.scmp.com/news/world/europe/article/3342251/ukraine-left-freezing-russia-bombs-energy-grid-peace-talks?utm_source=rss_feed</v>
+      </c>
+      <c r="C85" t="str">
+        <v>Ukraine left freezing as Russia bombs energy grid before peace talks</v>
+      </c>
+      <c r="D85" t="str">
+        <v>俄罗斯在和平谈判前轰炸乌克兰能源设施，导致乌克兰民众面临严寒，加剧人道危机。</v>
+      </c>
+      <c r="E85">
+        <v>5</v>
+      </c>
+      <c r="F85" t="str">
+        <v>normal</v>
+      </c>
+      <c r="G85" t="str">
+        <v>2026-02-03T10:56:10.149Z</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="str">
+        <v>国家紧急</v>
+      </c>
+      <c r="B86" t="str">
+        <v>https://www.scmp.com/news/world/europe/article/3342251/ukraine-left-freezing-russia-bombs-energy-grid-peace-talks?utm_source=rss_feed</v>
+      </c>
+      <c r="C86" t="str">
+        <v>Ukraine left freezing as Russia bombs energy grid before peace talks</v>
+      </c>
+      <c r="D86" t="str">
+        <v>分析失败</v>
+      </c>
+      <c r="E86" t="str">
+        <v/>
+      </c>
+      <c r="F86" t="str">
+        <v>normal</v>
+      </c>
+      <c r="G86" t="str">
+        <v>2026-02-03T10:56:10.149Z</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="str">
+        <v>国家紧急</v>
+      </c>
+      <c r="B87" t="str">
+        <v>https://www.scmp.com/news/world/europe/article/3342251/ukraine-left-freezing-russia-bombs-energy-grid-peace-talks?utm_source=rss_feed</v>
+      </c>
+      <c r="C87" t="str">
+        <v>Ukraine left freezing as Russia bombs energy grid before peace talks</v>
+      </c>
+      <c r="D87" t="str">
+        <v>在和平谈判前夕，俄罗斯轰炸乌克兰能源设施，导致乌克兰面临严寒，加剧人道危机。</v>
+      </c>
+      <c r="E87">
+        <v>5</v>
+      </c>
+      <c r="F87" t="str">
+        <v>normal</v>
+      </c>
+      <c r="G87" t="str">
+        <v>2026-02-03T10:56:10.149Z</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="str">
+        <v>国家紧急</v>
+      </c>
+      <c r="B88" t="str">
+        <v>https://www.scmp.com/news/world/europe/article/3342251/ukraine-left-freezing-russia-bombs-energy-grid-peace-talks?utm_source=rss_feed</v>
+      </c>
+      <c r="C88" t="str">
+        <v>Ukraine left freezing as Russia bombs energy grid before peace talks</v>
+      </c>
+      <c r="D88" t="str">
+        <v>在和平谈判前夕，俄罗斯轰炸乌克兰能源设施，导致乌克兰民众面临严寒，加剧人道主义危机。</v>
+      </c>
+      <c r="E88">
+        <v>5</v>
+      </c>
+      <c r="F88" t="str">
+        <v>normal</v>
+      </c>
+      <c r="G88" t="str">
+        <v>2026-02-03T10:56:10.149Z</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="str">
+        <v>国家紧急</v>
+      </c>
+      <c r="B89" t="str">
+        <v>https://www.rt.com/africa/631900-moscow-denounces-terrorist-attack-niger-airport/?utm_source=rss&amp;utm_medium=rss&amp;utm_campaign=RSS</v>
+      </c>
+      <c r="C89" t="str">
+        <v>Moscow denounces terrorist attack at Niger airport</v>
+      </c>
+      <c r="D89" t="str">
+        <v>莫斯科谴责尼日尔机场发生的恐怖袭击，具体细节未知。</v>
+      </c>
+      <c r="E89">
+        <v>3</v>
+      </c>
+      <c r="F89" t="str">
+        <v>normal</v>
+      </c>
+      <c r="G89" t="str">
+        <v>2026-02-03T10:56:10.149Z</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="str">
+        <v>国家紧急</v>
+      </c>
+      <c r="B90" t="str">
+        <v>https://www.zerohedge.com/markets/us-sanctioned-russian-military-transport-plane-touches-down-cuban-airfield</v>
+      </c>
+      <c r="C90" t="str">
+        <v>US-Sanctioned Russian Military Transport Plane Touches Down At Cuban Airfield</v>
+      </c>
+      <c r="D90" t="str">
+        <v>受美国制裁的俄罗斯军用运输机降落在古巴机场，可能引发美方关注和对俄古关系的质疑。</v>
+      </c>
+      <c r="E90">
+        <v>4</v>
+      </c>
+      <c r="F90" t="str">
+        <v>normal</v>
+      </c>
+      <c r="G90" t="str">
+        <v>2026-02-03T10:56:10.149Z</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="str">
+        <v>国家紧急</v>
+      </c>
+      <c r="B91" t="str">
+        <v>https://www.rt.com/africa/631900-moscow-denounces-terrorist-attack-niger-airport/?utm_source=rss&amp;utm_medium=rss&amp;utm_campaign=RSS</v>
+      </c>
+      <c r="C91" t="str">
+        <v>Moscow denounces terrorist attack at Niger airport</v>
+      </c>
+      <c r="D91" t="str">
+        <v>莫斯科谴责尼日尔机场发生的恐怖袭击事件，具体细节未知。</v>
+      </c>
+      <c r="E91">
+        <v>3</v>
+      </c>
+      <c r="F91" t="str">
+        <v>normal</v>
+      </c>
+      <c r="G91" t="str">
+        <v>2026-02-03T10:56:10.149Z</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="str">
+        <v>大宗商品波动</v>
+      </c>
+      <c r="B92" t="str">
+        <v>https://www.marketwatch.com/story/during-the-worst-day-for-gold-in-46-years-options-traders-made-bets-the-metal-could-hit-20-000-2b5393a4?mod=mw_rss_topstories</v>
+      </c>
+      <c r="C92" t="str">
+        <v>During the worst day for gold in 46 years, options traders made bets the metal could hit $20,000</v>
+      </c>
+      <c r="D92" t="str">
+        <v>金价暴跌日，期权交易员押注金价飙升至2万美元，反映市场投机情绪强烈，但风险极高。</v>
+      </c>
+      <c r="E92">
+        <v>3</v>
+      </c>
+      <c r="F92" t="str">
+        <v>normal</v>
+      </c>
+      <c r="G92" t="str">
+        <v>2026-02-03T10:56:10.149Z</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="str">
+        <v>大宗商品波动</v>
+      </c>
+      <c r="B93" t="str">
+        <v>https://www.marketwatch.com/story/im-spooked-do-gold-and-silver-belong-in-my-retirement-portfolio-after-their-dramatic-fall-in-value-a5bc4b3e?mod=mw_rss_topstories</v>
+      </c>
+      <c r="C93" t="str">
+        <v>‘I’m spooked’: Do gold and silver belong in my retirement portfolio after their dramatic fall in value?</v>
+      </c>
+      <c r="D93" t="str">
+        <v>金银价格大幅下跌后，投资者考虑是否应将其纳入退休投资组合，文章探讨了金银投资的风险与收益。</v>
+      </c>
+      <c r="E93">
+        <v>3</v>
+      </c>
+      <c r="F93" t="str">
+        <v>normal</v>
+      </c>
+      <c r="G93" t="str">
+        <v>2026-02-03T10:56:10.149Z</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="str">
+        <v>大宗商品波动</v>
+      </c>
+      <c r="B94" t="str">
+        <v>https://www.technologyreview.com/2026/02/03/1132047/microbes-extract-metal-cleantech/</v>
+      </c>
+      <c r="C94" t="str">
+        <v>Microbes could extract the metal needed for cleantech</v>
+      </c>
+      <c r="D94" t="str">
+        <v>微生物可能用于提取清洁技术所需的金属，为可持续资源获取提供新途径。</v>
+      </c>
+      <c r="E94">
+        <v>4</v>
+      </c>
+      <c r="F94" t="str">
+        <v>normal</v>
+      </c>
+      <c r="G94" t="str">
+        <v>2026-02-03T10:56:10.149Z</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="str">
+        <v>大宗商品波动</v>
+      </c>
+      <c r="B95" t="str">
+        <v>https://seekingalpha.com/article/4865184-gold-silver-and-equities-evidence-positive-volspot-correlation?source=feed_all_articles</v>
+      </c>
+      <c r="C95" t="str">
+        <v>Gold, Silver And Equities Evidence Positive Vol/Spot Correlation</v>
+      </c>
+      <c r="D95" t="str">
+        <v>分析失败</v>
+      </c>
+      <c r="E95" t="str">
+        <v/>
+      </c>
+      <c r="F95" t="str">
+        <v>normal</v>
+      </c>
+      <c r="G95" t="str">
+        <v>2026-02-03T10:56:10.149Z</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="str">
+        <v>大宗商品波动</v>
+      </c>
+      <c r="B96" t="str">
+        <v>https://www.technologyreview.com/2026/02/03/1132047/microbes-extract-metal-cleantech/</v>
+      </c>
+      <c r="C96" t="str">
+        <v>Microbes could extract the metal needed for cleantech</v>
+      </c>
+      <c r="D96" t="str">
+        <v>微生物可能用于提取清洁技术所需的金属，为可持续资源获取提供新途径。</v>
+      </c>
+      <c r="E96">
+        <v>4</v>
+      </c>
+      <c r="F96" t="str">
+        <v>normal</v>
+      </c>
+      <c r="G96" t="str">
+        <v>2026-02-03T10:56:10.149Z</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="str">
+        <v>大宗商品波动</v>
+      </c>
+      <c r="B97" t="str">
+        <v>https://finance.yahoo.com/news/eldorado-gold-acquire-foran-mining-102211341.html</v>
+      </c>
+      <c r="C97" t="str">
+        <v>Eldorado Gold to acquire Foran Mining in $2.78bn deal</v>
+      </c>
+      <c r="D97" t="str">
+        <v>Eldorado Gold以27.8亿美元收购Foran Mining，扩大其黄金和基本金属资产组合。</v>
+      </c>
+      <c r="E97">
+        <v>4</v>
+      </c>
+      <c r="F97" t="str">
+        <v>normal</v>
+      </c>
+      <c r="G97" t="str">
+        <v>2026-02-03T10:56:10.149Z</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="str">
+        <v>大宗商品波动</v>
+      </c>
+      <c r="B98" t="str">
+        <v>https://www.zerohedge.com/energy/polish-president-pushes-aggressive-move-nuclear-bypassing-lng-amidst-geopolitical-turmoils</v>
+      </c>
+      <c r="C98" t="str">
+        <v>Polish President Pushes For Aggressive Move To Nuclear, Bypassing LNG Amidst 'Geopolitical Turmoils'</v>
+      </c>
+      <c r="D98" t="str">
+        <v>波兰总统呼吁在“地缘政治动荡”中采取激进的核能发展策略，绕过液化天然气。</v>
+      </c>
+      <c r="E98">
+        <v>4</v>
+      </c>
+      <c r="F98" t="str">
+        <v>normal</v>
+      </c>
+      <c r="G98" t="str">
+        <v>2026-02-03T10:56:10.149Z</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="str">
+        <v>大宗商品波动</v>
+      </c>
+      <c r="B99" t="str">
+        <v>https://www.zerohedge.com/energy/polish-president-pushes-aggressive-move-nuclear-bypassing-lng-amidst-geopolitical-turmoils</v>
+      </c>
+      <c r="C99" t="str">
+        <v>Polish President Pushes For Aggressive Move To Nuclear, Bypassing LNG Amidst 'Geopolitical Turmoils'</v>
+      </c>
+      <c r="D99" t="str">
+        <v>分析失败</v>
+      </c>
+      <c r="E99" t="str">
+        <v/>
+      </c>
+      <c r="F99" t="str">
+        <v>normal</v>
+      </c>
+      <c r="G99" t="str">
+        <v>2026-02-03T10:56:10.149Z</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="str">
+        <v>大宗商品波动</v>
+      </c>
+      <c r="B100" t="str">
+        <v>https://finance.yahoo.com/news/buy-ishares-silver-trust-etf-090500582.html</v>
+      </c>
+      <c r="C100" t="str">
+        <v>Should You Buy the iShares Silver Trust ETF After Its Steep Sell-Off?</v>
+      </c>
+      <c r="D100" t="str">
+        <v>本文分析iShares Silver Trust ETF大幅抛售后是否值得买入，为投资者提供投资建议。</v>
+      </c>
+      <c r="E100">
+        <v>3</v>
+      </c>
+      <c r="F100" t="str">
+        <v>normal</v>
+      </c>
+      <c r="G100" t="str">
+        <v>2026-02-03T10:56:10.149Z</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="str">
+        <v>大宗商品波动</v>
+      </c>
+      <c r="B101" t="str">
+        <v>https://finance.yahoo.com/news/worst-day-silver-46-years-091100399.html</v>
+      </c>
+      <c r="C101" t="str">
+        <v>The Worst Day for Silver in 46 Years Serves as a Warning for the Stock Market's 2 Hottest Trends: AI and Quantum Computing</v>
+      </c>
+      <c r="D101" t="str">
+        <v>白银暴跌预示AI和量子计算领域可能存在过热风险，投资者需警惕市场回调。</v>
+      </c>
+      <c r="E101">
+        <v>3</v>
+      </c>
+      <c r="F101" t="str">
+        <v>normal</v>
+      </c>
+      <c r="G101" t="str">
+        <v>2026-02-03T10:56:10.149Z</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="str">
+        <v>市场异常</v>
+      </c>
+      <c r="B102" t="str">
+        <v>https://in-cyprus.philenews.com/local/university-cyprus-construction-delays-72-months-cost-overrun-auditor-general/</v>
+      </c>
+      <c r="C102" t="str">
+        <v>UCY construction projects delayed by six years as costs surge €15.2m</v>
+      </c>
+      <c r="D102" t="str">
+        <v>塞浦路斯大学(UCY)建设项目因成本增加1520万欧元而延误六年。</v>
+      </c>
+      <c r="E102">
+        <v>3</v>
+      </c>
+      <c r="F102" t="str">
+        <v>normal</v>
+      </c>
+      <c r="G102" t="str">
+        <v>2026-02-03T10:56:10.149Z</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="str">
+        <v>市场异常</v>
+      </c>
+      <c r="B103" t="str">
+        <v>https://cyprus-mail.com/2026/02/03/global-air-passenger-demand-hit-record-highs-in-2025</v>
+      </c>
+      <c r="C103" t="str">
+        <v>Global air passenger demand hit record highs in 2025</v>
+      </c>
+      <c r="D103" t="str">
+        <v>2025年全球航空客运需求创历史新高，表明航空业持续复苏和增长。</v>
+      </c>
+      <c r="E103">
+        <v>4</v>
+      </c>
+      <c r="F103" t="str">
+        <v>normal</v>
+      </c>
+      <c r="G103" t="str">
+        <v>2026-02-03T10:56:10.149Z</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="str">
+        <v>市场异常</v>
+      </c>
+      <c r="B104" t="str">
+        <v>https://cyprus-mail.com/2026/02/03/global-air-passenger-demand-hit-record-highs-in-2025</v>
+      </c>
+      <c r="C104" t="str">
+        <v>Global air passenger demand hit record highs in 2025</v>
+      </c>
+      <c r="D104" t="str">
+        <v>2025年全球航空客运需求创历史新高，表明航空业持续复苏和增长。</v>
+      </c>
+      <c r="E104">
+        <v>4</v>
+      </c>
+      <c r="F104" t="str">
+        <v>normal</v>
+      </c>
+      <c r="G104" t="str">
+        <v>2026-02-03T10:56:10.149Z</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="str">
+        <v>市场异常</v>
+      </c>
+      <c r="B105" t="str">
+        <v>https://cyprus-mail.com/2026/02/03/global-air-passenger-demand-hit-record-highs-in-2025</v>
+      </c>
+      <c r="C105" t="str">
+        <v>Global air passenger demand hit record highs in 2025</v>
+      </c>
+      <c r="D105" t="str">
+        <v>2025年全球航空客运需求创历史新高，反映了旅游业的强劲复苏和增长。（29字）</v>
+      </c>
+      <c r="E105">
+        <v>4</v>
+      </c>
+      <c r="F105" t="str">
+        <v>normal</v>
+      </c>
+      <c r="G105" t="str">
+        <v>2026-02-03T10:56:10.149Z</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="str">
+        <v>市场异常</v>
+      </c>
+      <c r="B106" t="str">
+        <v>https://in-cyprus.philenews.com/local/cyprus-state-hospitals-exceed-capacity-respiratory-illnesses-ae-waits-24-hours/</v>
+      </c>
+      <c r="C106" t="str">
+        <v>Hospitals exceed capacity as respiratory illnesses surge, patients wait over 24 hours in A&amp;E</v>
+      </c>
+      <c r="D106" t="str">
+        <v>呼吸道疾病激增导致医院超负荷运转，急诊患者等待时间超过24小时，医疗系统面临巨大压力。</v>
+      </c>
+      <c r="E106">
+        <v>5</v>
+      </c>
+      <c r="F106" t="str">
+        <v>normal</v>
+      </c>
+      <c r="G106" t="str">
+        <v>2026-02-03T10:56:10.149Z</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="str">
+        <v>市场异常</v>
+      </c>
+      <c r="B107" t="str">
+        <v>https://finance.yahoo.com/news/byd-global-sales-plunge-30-092955748.html</v>
+      </c>
+      <c r="C107" t="str">
+        <v>BYD’s global sales plunge 30% in January</v>
+      </c>
+      <c r="D107" t="str">
+        <v>比亚迪1月全球销量暴跌30%，或受季节性因素及市场竞争影响。</v>
+      </c>
+      <c r="E107">
+        <v>4</v>
+      </c>
+      <c r="F107" t="str">
+        <v>normal</v>
+      </c>
+      <c r="G107" t="str">
+        <v>2026-02-03T10:56:10.149Z</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="str">
+        <v>市场异常</v>
+      </c>
+      <c r="B108" t="str">
+        <v>https://finance.yahoo.com/news/singapore-air-show-kicks-off-081650251.html</v>
+      </c>
+      <c r="C108" t="str">
+        <v>Singapore air show kicks off amid supply chain strains, regional demand surge</v>
+      </c>
+      <c r="D108" t="str">
+        <v>新加坡航展在供应链紧张和区域需求激增的背景下开幕，凸显航空业面临的挑战与机遇。</v>
+      </c>
+      <c r="E108">
+        <v>4</v>
+      </c>
+      <c r="F108" t="str">
+        <v>normal</v>
+      </c>
+      <c r="G108" t="str">
+        <v>2026-02-03T10:56:10.149Z</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="str">
+        <v>市场异常</v>
+      </c>
+      <c r="B109" t="str">
+        <v>https://www.bbc.com/news/articles/c8e5zwndddyo?at_medium=RSS&amp;at_campaign=rss</v>
+      </c>
+      <c r="C109" t="str">
+        <v>Air India grounds Boeing jet after pilot flags possible fuel control switch defect</v>
+      </c>
+      <c r="D109" t="str">
+        <v>印度航空因飞行员报告潜在燃油控制开关缺陷，停飞一架波音飞机进行检查，保障飞行安全。</v>
+      </c>
+      <c r="E109">
+        <v>4</v>
+      </c>
+      <c r="F109" t="str">
+        <v>normal</v>
+      </c>
+      <c r="G109" t="str">
+        <v>2026-02-03T10:56:10.149Z</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="str">
+        <v>市场异常</v>
+      </c>
+      <c r="B110" t="str">
+        <v>https://www.bbc.com/news/articles/c8e5zwndddyo?at_medium=RSS&amp;at_campaign=rss</v>
+      </c>
+      <c r="C110" t="str">
+        <v>Air India grounds Boeing jet after pilot flags possible fuel control switch defect</v>
+      </c>
+      <c r="D110" t="str">
+        <v>印度航空因飞行员报告潜在燃油控制开关故障，停飞一架波音飞机进行检查。</v>
+      </c>
+      <c r="E110">
+        <v>3</v>
+      </c>
+      <c r="F110" t="str">
+        <v>normal</v>
+      </c>
+      <c r="G110" t="str">
+        <v>2026-02-03T10:56:10.149Z</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="str">
+        <v>市场异常</v>
+      </c>
+      <c r="B111" t="str">
+        <v>https://www.scmp.com/news/hong-kong/society/article/3342216/data-leaks-jump-21-hong-kong-doxxing-hits-record-low?utm_source=rss_feed</v>
+      </c>
+      <c r="C111" t="str">
+        <v>Data leaks jump 21% in Hong Kong, doxxing cases hit record low</v>
+      </c>
+      <c r="D111" t="str">
+        <v>香港数据泄露事件激增21%，但人肉搜索案件数量降至历史新低，反映网络安全形势变化。</v>
+      </c>
+      <c r="E111">
+        <v>4</v>
+      </c>
+      <c r="F111" t="str">
+        <v>normal</v>
+      </c>
+      <c r="G111" t="str">
+        <v>2026-02-03T10:56:10.149Z</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:G21"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:G111"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>